<commit_message>
visualizando produtos ativos e inativos.
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -22,28 +22,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="410">
   <si>
-    <t xml:space="preserve">Produto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Interno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descrição</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data de Criação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inativo?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código Integração</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantidade p/ Embalagem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor</t>
+    <t xml:space="preserve">produto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod_interno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descricao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_criacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod_integracao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qde_embalagem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor</t>
   </si>
   <si>
     <t xml:space="preserve">Produto 1</t>
@@ -1395,22 +1395,22 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>